<commit_message>
Modified template config files to have labels for traits, models in order to have better labeling in plots.
</commit_message>
<xml_diff>
--- a/Workflows/templates/configs/model-traits.cfg.xlsx
+++ b/Workflows/templates/configs/model-traits.cfg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewmaule/Documents/personal/education/UW-Madison/Zalapa/projects/CNJ0x-Trait-Mapping/Workflows/templates/configs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewmaule/Documents/personal/education/UW-Madison/Zalapa/projects/CNJ0x-Trait-Mapping/Workflows/9/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B136944-00C1-5244-9ADE-4512065AC00E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5748B3-4014-4142-962D-0CEA12C6FCEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model-traits.cfg" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="39">
   <si>
     <t>model</t>
   </si>
@@ -96,10 +96,58 @@
     <t>description</t>
   </si>
   <si>
-    <t>~vs(id, Gu=A) + id:year</t>
-  </si>
-  <si>
-    <t>~vs(id, Gu=A)</t>
+    <t>~vs(id, Gu=A)+vs(rowf)+vs(columnf)+vs(spl2D(row,column))</t>
+  </si>
+  <si>
+    <t>~vs(id, Gu=A) + id:year + vs(rowf)+vs(columnf)+vs(spl2D(row,column))</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Berry Length</t>
+  </si>
+  <si>
+    <t>Berry Width</t>
+  </si>
+  <si>
+    <t>Berry Weight</t>
+  </si>
+  <si>
+    <t>Number of Seeds</t>
+  </si>
+  <si>
+    <t>Number of Pedicels</t>
+  </si>
+  <si>
+    <t>Number of Berries</t>
+  </si>
+  <si>
+    <t>Total Berry Weight</t>
+  </si>
+  <si>
+    <t>label_short</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>TBM</t>
   </si>
 </sst>
 </file>
@@ -940,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,14 +999,17 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.33203125" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -987,10 +1038,16 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -1006,7 +1063,7 @@
         <v>berry_length~1</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -1014,8 +1071,14 @@
       <c r="H2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -1031,7 +1094,7 @@
         <v>berry_width~1</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -1039,8 +1102,14 @@
       <c r="H3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -1056,7 +1125,7 @@
         <v>berry_weight~1</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -1064,8 +1133,14 @@
       <c r="H4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -1081,7 +1156,7 @@
         <v>num_seeds~1</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -1089,8 +1164,14 @@
       <c r="H5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -1106,7 +1187,7 @@
         <v>num_peds~1</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -1114,11 +1195,14 @@
       <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -1134,16 +1218,19 @@
         <v>num_berries~1</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -1159,13 +1246,19 @@
         <v>total_berry_weight~1</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2012</v>
       </c>
@@ -1181,7 +1274,7 @@
         <v>berry_length~1</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -1189,8 +1282,14 @@
       <c r="H9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -1206,7 +1305,7 @@
         <v>berry_width~1</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -1214,8 +1313,14 @@
       <c r="H10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -1231,7 +1336,7 @@
         <v>berry_weight~1</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1239,8 +1344,14 @@
       <c r="H11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -1256,7 +1367,7 @@
         <v>num_seeds~1</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -1264,8 +1375,14 @@
       <c r="H12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2012</v>
       </c>
@@ -1281,7 +1398,7 @@
         <v>num_peds~1</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -1289,8 +1406,14 @@
       <c r="H13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -1306,16 +1429,19 @@
         <v>num_berries~1</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
       </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2012</v>
       </c>
@@ -1331,13 +1457,19 @@
         <v>total_berry_weight~1</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2013</v>
       </c>
@@ -1353,7 +1485,7 @@
         <v>berry_length~1</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
@@ -1361,8 +1493,14 @@
       <c r="H16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -1378,7 +1516,7 @@
         <v>berry_width~1</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -1386,11 +1524,14 @@
       <c r="H17" t="s">
         <v>10</v>
       </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -1406,7 +1547,7 @@
         <v>berry_weight~1</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
@@ -1414,8 +1555,14 @@
       <c r="H18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2013</v>
       </c>
@@ -1431,7 +1578,7 @@
         <v>num_seeds~1</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1439,8 +1586,14 @@
       <c r="H19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -1456,7 +1609,7 @@
         <v>num_peds~1</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -1464,8 +1617,14 @@
       <c r="H20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -1481,16 +1640,19 @@
         <v>num_berries~1</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2013</v>
       </c>
@@ -1506,16 +1668,19 @@
         <v>total_berry_weight~1</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
       </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1527,7 +1692,7 @@
         <v>berry_length~year</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
@@ -1535,8 +1700,14 @@
       <c r="H23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1548,7 +1719,7 @@
         <v>berry_width~year</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
@@ -1556,8 +1727,14 @@
       <c r="H24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1569,7 +1746,7 @@
         <v>berry_weight~year</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
         <v>9</v>
@@ -1577,8 +1754,14 @@
       <c r="H25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1590,7 +1773,7 @@
         <v>num_seeds~year</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -1598,8 +1781,14 @@
       <c r="H26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1611,7 +1800,7 @@
         <v>num_peds~year</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F27" t="s">
         <v>9</v>
@@ -1619,8 +1808,14 @@
       <c r="H27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1632,13 +1827,19 @@
         <v>num_berries~year</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1650,10 +1851,16 @@
         <v>total_berry_weight~year</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
         <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing model-trait.cfg.* files to add entries for model_label, label (trait), and label_short (abbreviated descriptor for trait).
</commit_message>
<xml_diff>
--- a/Workflows/templates/configs/model-traits.cfg.xlsx
+++ b/Workflows/templates/configs/model-traits.cfg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewmaule/Documents/personal/education/UW-Madison/Zalapa/projects/CNJ0x-Trait-Mapping/Workflows/9/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5748B3-4014-4142-962D-0CEA12C6FCEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F58321-E31D-9448-A6C9-F8F34B54F309}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="41">
   <si>
     <t>model</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>TBM</t>
+  </si>
+  <si>
+    <t>model_label</t>
+  </si>
+  <si>
+    <t>All Years</t>
   </si>
 </sst>
 </file>
@@ -988,878 +994,986 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="63.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2011</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <f>A2</f>
+        <v>2011</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <f>_xlfn.CONCAT("year == '",A2,"'")</f>
         <v>year == '2011'</v>
       </c>
-      <c r="D2" t="str">
-        <f>_xlfn.CONCAT(B2,"~1")</f>
+      <c r="E2" t="str">
+        <f>_xlfn.CONCAT(C2,"~1")</f>
         <v>berry_length~1</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">A3</f>
+        <v>2011</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C22" si="0">_xlfn.CONCAT("year == '",A3,"'")</f>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D22" si="1">_xlfn.CONCAT("year == '",A3,"'")</f>
         <v>year == '2011'</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D22" si="1">_xlfn.CONCAT(B3,"~1")</f>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E22" si="2">_xlfn.CONCAT(C3,"~1")</f>
         <v>berry_width~1</v>
       </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2011</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2011'</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2011'</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
         <v>berry_weight~1</v>
       </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>26</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2011'</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2011'</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
         <v>num_seeds~1</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>27</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2011</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2011'</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2011'</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
         <v>num_peds~1</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
         <v>15</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2011</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2011'</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2011'</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
         <v>num_berries~1</v>
       </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" t="s">
         <v>29</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2011</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2011'</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2011'</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
         <v>total_berry_weight~1</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
       <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
         <v>30</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2012</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
         <v>berry_length~1</v>
       </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
       <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
         <v>10</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>24</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2012</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
         <v>berry_width~1</v>
       </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2012</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
         <v>berry_weight~1</v>
       </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
       <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>26</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2012</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
         <v>num_seeds~1</v>
       </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
         <v>10</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>27</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2012</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
         <v>num_peds~1</v>
       </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
       <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
         <v>15</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>28</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2012</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
         <v>num_berries~1</v>
       </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
       <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" t="s">
         <v>29</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2012</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2012'</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2012'</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
         <v>total_berry_weight~1</v>
       </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
       <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s">
         <v>30</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2013</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C16" t="s">
         <v>8</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
         <v>berry_length~1</v>
       </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
       <c r="F16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
         <v>10</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>24</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2013</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C17" t="s">
         <v>11</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
         <v>berry_width~1</v>
       </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
       <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
         <v>10</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>25</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2013</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
         <v>berry_weight~1</v>
       </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
       <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
         <v>10</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>26</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2013</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C19" t="s">
         <v>13</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
         <v>num_seeds~1</v>
       </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
       <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
         <v>10</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>27</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2013</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C20" t="s">
         <v>14</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
         <v>num_peds~1</v>
       </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
       <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
         <v>15</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>28</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2013</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C21" t="s">
         <v>16</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
         <v>num_berries~1</v>
       </c>
-      <c r="E21" t="s">
-        <v>21</v>
-      </c>
       <c r="F21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" t="s">
         <v>29</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2013</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="C22" t="s">
         <v>17</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>year == '2013'</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
+        <v>year == '2013'</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
         <v>total_berry_weight~1</v>
       </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
       <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" t="s">
         <v>30</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
       <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D23" t="str">
-        <f>_xlfn.CONCAT(B23,"~year")</f>
+      <c r="E23" t="str">
+        <f>_xlfn.CONCAT(C23,"~year")</f>
         <v>berry_length~year</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" t="s">
         <v>10</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>24</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="str">
-        <f t="shared" ref="D24:D29" si="2">_xlfn.CONCAT(B24,"~year")</f>
+      <c r="E24" t="str">
+        <f t="shared" ref="E24:E29" si="3">_xlfn.CONCAT(C24,"~year")</f>
         <v>berry_width~year</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>22</v>
       </c>
-      <c r="F24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" t="s">
         <v>10</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>25</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
       <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" si="2"/>
+      <c r="E25" t="str">
+        <f t="shared" si="3"/>
         <v>berry_weight~year</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>22</v>
       </c>
-      <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" t="s">
         <v>10</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>26</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
       <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" t="str">
-        <f t="shared" si="2"/>
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
         <v>num_seeds~year</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>22</v>
       </c>
-      <c r="F26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" t="s">
         <v>10</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>27</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" si="2"/>
+      <c r="E27" t="str">
+        <f t="shared" si="3"/>
         <v>num_peds~year</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>22</v>
       </c>
-      <c r="F27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" t="s">
         <v>15</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>28</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
       <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
         <v>16</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="2"/>
+      <c r="E28" t="str">
+        <f t="shared" si="3"/>
         <v>num_berries~year</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>22</v>
       </c>
-      <c r="F28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" t="s">
         <v>29</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
       <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
         <v>17</v>
       </c>
-      <c r="D29" t="str">
-        <f t="shared" si="2"/>
+      <c r="E29" t="str">
+        <f t="shared" si="3"/>
         <v>total_berry_weight~year</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>22</v>
       </c>
-      <c r="F29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" t="s">
         <v>30</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>